<commit_message>
Negative delivery test cases added
</commit_message>
<xml_diff>
--- a/tests/artifact/script/DeliveryNote.xlsx
+++ b/tests/artifact/script/DeliveryNote.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="830">
   <si>
     <t>target</t>
   </si>
@@ -2352,7 +2352,7 @@
     <t>your name</t>
   </si>
   <si>
-    <t>Negative - /log</t>
+    <t>Negative - /log/</t>
   </si>
   <si>
     <t>gkToken</t>
@@ -2401,7 +2401,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>Positive - /log</t>
+    <t>Positive - /log/</t>
   </si>
   <si>
     <t>Set headers for Authorization</t>
@@ -2597,7 +2597,13 @@
     <t>Positive - Create DeliveryNote</t>
   </si>
   <si>
+    <t>Negative - /log</t>
+  </si>
+  <si>
     <t>${api.baseUrl}delchal/${delete_dcid}</t>
+  </si>
+  <si>
+    <t>Positive - /log</t>
   </si>
 </sst>
 </file>
@@ -2605,11 +2611,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -3188,16 +3194,16 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3451,7 +3457,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -26583,8 +26589,8 @@
   <sheetPr/>
   <dimension ref="A1:O204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
@@ -35463,7 +35469,7 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A5" s="19" t="s">
-        <v>761</v>
+        <v>827</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>814</v>
@@ -35502,7 +35508,7 @@
         <v>765</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="G6" s="27"/>
       <c r="H6" s="29"/>
@@ -35639,7 +35645,7 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A12" s="19" t="s">
-        <v>775</v>
+        <v>829</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>776</v>
@@ -39560,7 +39566,7 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A5" s="19" t="s">
-        <v>761</v>
+        <v>827</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>814</v>
@@ -39736,7 +39742,7 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A12" s="19" t="s">
-        <v>775</v>
+        <v>829</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>776</v>

</xml_diff>